<commit_message>
Allow / or - as date separator.  Require date to have a year 2000-2999. Update XLSX template instructions to tell user to type ' before dates.
</commit_message>
<xml_diff>
--- a/app/resources/notes-template.xlsx
+++ b/app/resources/notes-template.xlsx
@@ -96,13 +96,6 @@
     <t>full_name</t>
   </si>
   <si>
-    <t>Date &amp; time that you are entering this row.   yyyy-mm-dd hh:mm format is required.
-In Excel, type:
-    CTRL+;  (semicolon)
-    then SPACE
-    then CTRL+:  (colon)</t>
-  </si>
-  <si>
     <t>mary.example@gmail.com</t>
   </si>
   <si>
@@ -189,6 +182,13 @@
   - believed_missing
   - is_note_author
 "is_note_author" is for a person posting about him/herself.</t>
+  </si>
+  <si>
+    <t>Date &amp; time that you are entering this row. Must use yyyy-mm-dd hh:mm format. In Excel, type:
+    '  (apostrophe)
+    then CTRL+;  (semicolon)
+    then SPACE
+    then CTRL+:  (colon)</t>
   </si>
 </sst>
 </file>
@@ -270,7 +270,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
@@ -328,6 +328,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -666,7 +670,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
@@ -679,7 +683,7 @@
   <cols>
     <col min="1" max="1" width="48.33203125" style="15" customWidth="1"/>
     <col min="2" max="2" width="18" style="15" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" style="5" customWidth="1"/>
     <col min="4" max="4" width="18" style="5" customWidth="1"/>
     <col min="5" max="5" width="22.83203125" style="5" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" style="5" customWidth="1"/>
@@ -693,7 +697,7 @@
   <sheetData>
     <row r="1" spans="1:18" s="7" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>21</v>
@@ -712,22 +716,22 @@
       </c>
       <c r="P1" s="17"/>
       <c r="Q1" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="R1" s="17" t="s">
         <v>46</v>
-      </c>
-      <c r="R1" s="17" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="7" customFormat="1" ht="45" customHeight="1">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="1">
         <v>8</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -778,31 +782,31 @@
     </row>
     <row r="4" spans="1:18" s="13" customFormat="1" ht="135">
       <c r="A4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>51</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>20</v>
@@ -857,22 +861,22 @@
         <v>22</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" s="5" t="b">
         <v>1</v>
@@ -881,48 +885,48 @@
         <v>13</v>
       </c>
       <c r="J6" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" s="5" t="s">
         <v>12</v>
@@ -930,25 +934,25 @@
     </row>
     <row r="8" spans="1:18" ht="45">
       <c r="A8" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="C8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H8" s="5" t="b">
         <v>0</v>
@@ -957,15 +961,18 @@
         <v>11</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="C9" s="19"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I6:I1048576">
       <formula1>$M$1:$O$1</formula1>
     </dataValidation>

</xml_diff>